<commit_message>
Everything works. A lot of spaghetti code
</commit_message>
<xml_diff>
--- a/obrazec.xlsx
+++ b/obrazec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programming\Python\Accountant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC97A37-79E0-471C-ABD8-572BCE50BD03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3CB49D-5B6A-4F60-8CF4-4D73CA20E98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="76">
   <si>
     <t xml:space="preserve">До </t>
   </si>
@@ -888,6 +888,63 @@
       </rPr>
       <t>"Код в СЕБРА/идентификатор за централизация на титуляря".</t>
     </r>
+  </si>
+  <si>
+    <t>н</t>
+  </si>
+  <si>
+    <t>Н</t>
+  </si>
+  <si>
+    <t>а</t>
+  </si>
+  <si>
+    <t>ц</t>
+  </si>
+  <si>
+    <t>и</t>
+  </si>
+  <si>
+    <t>о</t>
+  </si>
+  <si>
+    <t>л</t>
+  </si>
+  <si>
+    <t>г</t>
+  </si>
+  <si>
+    <t>е</t>
+  </si>
+  <si>
+    <t>я</t>
+  </si>
+  <si>
+    <t>з</t>
+  </si>
+  <si>
+    <t>п</t>
+  </si>
+  <si>
+    <t>р</t>
+  </si>
+  <si>
+    <t>х</t>
+  </si>
+  <si>
+    <t>д</t>
+  </si>
+  <si>
+    <t>т</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -1863,7 +1920,7 @@
   <dimension ref="A1:AK69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2559,37 +2616,93 @@
     </row>
     <row r="18" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
+      <c r="B18" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="11"/>
-      <c r="S18" s="11"/>
+      <c r="M18" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="N18" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="O18" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="P18" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q18" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="R18" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="S18" s="11" t="s">
+        <v>66</v>
+      </c>
       <c r="T18" s="11"/>
-      <c r="U18" s="11"/>
-      <c r="V18" s="11"/>
+      <c r="U18" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="V18" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="W18" s="11"/>
-      <c r="X18" s="11"/>
-      <c r="Y18" s="11"/>
-      <c r="Z18" s="11"/>
-      <c r="AA18" s="11"/>
-      <c r="AB18" s="11"/>
-      <c r="AC18" s="11"/>
-      <c r="AD18" s="11"/>
-      <c r="AE18" s="11"/>
-      <c r="AF18" s="11"/>
+      <c r="X18" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y18" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z18" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA18" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB18" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC18" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD18" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE18" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF18" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="AG18" s="11"/>
       <c r="AH18" s="11"/>
       <c r="AI18" s="11"/>
@@ -2823,9 +2936,15 @@
       <c r="S24" s="88"/>
       <c r="T24" s="88"/>
       <c r="U24" s="89"/>
-      <c r="V24" s="48"/>
-      <c r="W24" s="45"/>
-      <c r="X24" s="45"/>
+      <c r="V24" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="W24" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="X24" s="45" t="s">
+        <v>75</v>
+      </c>
       <c r="Y24" s="45"/>
       <c r="Z24" s="45"/>
       <c r="AA24" s="45"/>

</xml_diff>